<commit_message>
Bug fix (no ticket #): Implicit Collections Processing: Fix the case when a collection to process implicitly has its name as a substring of another identifier in the expression.
</commit_message>
<xml_diff>
--- a/jett-core/templates/ImplCollProcessingTemplate.xlsx
+++ b/jett-core/templates/ImplCollProcessingTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="17115" windowHeight="10230" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="17115" windowHeight="10230"/>
   </bookViews>
   <sheets>
     <sheet name="Implicit" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="groupDirCols" sheetId="13" r:id="rId10"/>
     <sheet name="indexVar" sheetId="14" r:id="rId11"/>
     <sheet name="limit" sheetId="15" r:id="rId12"/>
+    <sheet name="CollNameReplace" sheetId="16" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="63">
   <si>
     <t>City</t>
   </si>
@@ -178,6 +179,67 @@
   </si>
   <si>
     <t>${divisionsList.teams.city}?@limit=3</t>
+  </si>
+  <si>
+    <t>Counties</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Year Established</t>
+  </si>
+  <si>
+    <t>County Seat</t>
+  </si>
+  <si>
+    <t>FIPS Code</t>
+  </si>
+  <si>
+    <r>
+      <t>Area (km</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>${county.name}</t>
+  </si>
+  <si>
+    <t>${county.population}</t>
+  </si>
+  <si>
+    <t>${county.area}</t>
+  </si>
+  <si>
+    <t>${county.establishedYear}</t>
+  </si>
+  <si>
+    <t>${county.countySeat}</t>
+  </si>
+  <si>
+    <t>${county.fipsCode}</t>
   </si>
 </sst>
 </file>
@@ -187,7 +249,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +259,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -224,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -247,11 +318,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -259,6 +367,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -763,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -821,6 +942,83 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>